<commit_message>
Updated Contact Page, Home, and dependencies - improved design and functionality
</commit_message>
<xml_diff>
--- a/public/contact-backend/form-data.xlsx
+++ b/public/contact-backend/form-data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -582,9 +582,49 @@
         <v>6/23/2025, 1:37:39 PM</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>karthika</v>
+      </c>
+      <c r="B10" t="str">
+        <v>karthi@gmail.com</v>
+      </c>
+      <c r="C10" t="str">
+        <v>895</v>
+      </c>
+      <c r="D10" t="str">
+        <v>hh</v>
+      </c>
+      <c r="E10" t="str">
+        <v>btl</v>
+      </c>
+      <c r="F10" t="str">
+        <v>6/28/2025, 4:28:29 PM</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>xnbZ Xnb X</v>
+      </c>
+      <c r="B11" t="str">
+        <v>madhumitha.24mca@kct.ac.in</v>
+      </c>
+      <c r="C11" t="str">
+        <v>09865856968</v>
+      </c>
+      <c r="D11" t="str">
+        <v>ss</v>
+      </c>
+      <c r="E11" t="str">
+        <v>branding</v>
+      </c>
+      <c r="F11" t="str">
+        <v>6/28/2025, 5:05:03 PM</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>